<commit_message>
Corrected Tenure leave Issues
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/EffectiveDate.xlsx
+++ b/src/main/resources/TestData/EffectiveDate.xlsx
@@ -21,6 +21,7 @@
     <sheet name="Test" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">All_Scenarios_LTB!$A$1:$U$165</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">All_Without_Probation!$A$1:$T$83</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -5450,6 +5451,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -5463,13 +5468,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.5"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16221,11 +16226,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="7" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="7" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="7" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="7" width="7.83163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20402,9 +20407,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20488,24 +20493,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:U165"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A164" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B166" activeCellId="0" sqref="B166"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.5"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20573,7 +20578,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="68.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -20581,7 +20586,7 @@
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>354</v>
@@ -20963,7 +20968,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -20971,7 +20976,7 @@
         <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>360</v>
@@ -21028,7 +21033,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -21036,7 +21041,7 @@
         <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>361</v>
@@ -21093,7 +21098,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -21101,7 +21106,7 @@
         <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>362</v>
@@ -21158,7 +21163,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -21166,7 +21171,7 @@
         <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>363</v>
@@ -21223,7 +21228,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -21231,7 +21236,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>364</v>
@@ -21288,7 +21293,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -21296,7 +21301,7 @@
         <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>365</v>
@@ -21353,7 +21358,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -21361,7 +21366,7 @@
         <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>366</v>
@@ -21418,7 +21423,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -21426,7 +21431,7 @@
         <v>51</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>367</v>
@@ -21483,7 +21488,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -21491,7 +21496,7 @@
         <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>368</v>
@@ -21548,7 +21553,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -21556,7 +21561,7 @@
         <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>369</v>
@@ -21613,7 +21618,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -21621,7 +21626,7 @@
         <v>57</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>370</v>
@@ -21678,7 +21683,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -21686,7 +21691,7 @@
         <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>371</v>
@@ -21743,7 +21748,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -21751,7 +21756,7 @@
         <v>61</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>372</v>
@@ -21808,7 +21813,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -21816,7 +21821,7 @@
         <v>63</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>373</v>
@@ -21873,7 +21878,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -21881,7 +21886,7 @@
         <v>65</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>374</v>
@@ -21938,7 +21943,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -21946,7 +21951,7 @@
         <v>67</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>375</v>
@@ -22003,7 +22008,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -22011,7 +22016,7 @@
         <v>69</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>376</v>
@@ -22068,7 +22073,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -22076,7 +22081,7 @@
         <v>71</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>377</v>
@@ -22133,7 +22138,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -22141,7 +22146,7 @@
         <v>73</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>378</v>
@@ -22198,7 +22203,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -22206,7 +22211,7 @@
         <v>75</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>379</v>
@@ -22263,7 +22268,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>21</v>
       </c>
@@ -22271,7 +22276,7 @@
         <v>77</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>380</v>
@@ -22328,7 +22333,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
@@ -22336,7 +22341,7 @@
         <v>79</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>381</v>
@@ -22393,7 +22398,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>21</v>
       </c>
@@ -22401,7 +22406,7 @@
         <v>81</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>382</v>
@@ -22458,7 +22463,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>21</v>
       </c>
@@ -22466,7 +22471,7 @@
         <v>83</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>383</v>
@@ -22523,7 +22528,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
@@ -22531,7 +22536,7 @@
         <v>85</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>384</v>
@@ -22588,7 +22593,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>21</v>
       </c>
@@ -22596,7 +22601,7 @@
         <v>87</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>385</v>
@@ -22653,7 +22658,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>21</v>
       </c>
@@ -22661,7 +22666,7 @@
         <v>89</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>386</v>
@@ -22718,7 +22723,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>21</v>
       </c>
@@ -22726,7 +22731,7 @@
         <v>91</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>387</v>
@@ -22783,7 +22788,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>21</v>
       </c>
@@ -22791,7 +22796,7 @@
         <v>93</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>388</v>
@@ -22848,7 +22853,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -22856,7 +22861,7 @@
         <v>95</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>389</v>
@@ -22913,7 +22918,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>21</v>
       </c>
@@ -22921,7 +22926,7 @@
         <v>97</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>390</v>
@@ -22978,7 +22983,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>21</v>
       </c>
@@ -22986,7 +22991,7 @@
         <v>99</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>391</v>
@@ -23043,7 +23048,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>21</v>
       </c>
@@ -23051,7 +23056,7 @@
         <v>101</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>392</v>
@@ -23108,7 +23113,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>21</v>
       </c>
@@ -23116,7 +23121,7 @@
         <v>103</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>393</v>
@@ -23173,7 +23178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>21</v>
       </c>
@@ -23181,7 +23186,7 @@
         <v>105</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>394</v>
@@ -23238,7 +23243,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>21</v>
       </c>
@@ -23246,7 +23251,7 @@
         <v>107</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>395</v>
@@ -23303,7 +23308,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>21</v>
       </c>
@@ -23311,7 +23316,7 @@
         <v>109</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>396</v>
@@ -23368,7 +23373,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>21</v>
       </c>
@@ -23376,7 +23381,7 @@
         <v>111</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>397</v>
@@ -23433,7 +23438,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>21</v>
       </c>
@@ -23441,7 +23446,7 @@
         <v>113</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>398</v>
@@ -23498,7 +23503,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>21</v>
       </c>
@@ -23506,7 +23511,7 @@
         <v>115</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>399</v>
@@ -23563,7 +23568,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>21</v>
       </c>
@@ -23571,7 +23576,7 @@
         <v>117</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>400</v>
@@ -23628,7 +23633,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>21</v>
       </c>
@@ -23636,7 +23641,7 @@
         <v>119</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>401</v>
@@ -23693,7 +23698,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>21</v>
       </c>
@@ -23701,7 +23706,7 @@
         <v>121</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>402</v>
@@ -23758,7 +23763,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>21</v>
       </c>
@@ -23766,7 +23771,7 @@
         <v>123</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>403</v>
@@ -23823,7 +23828,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>21</v>
       </c>
@@ -23831,7 +23836,7 @@
         <v>125</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>404</v>
@@ -23888,7 +23893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>21</v>
       </c>
@@ -23896,7 +23901,7 @@
         <v>127</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>405</v>
@@ -23953,7 +23958,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>21</v>
       </c>
@@ -23961,7 +23966,7 @@
         <v>129</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>406</v>
@@ -24018,7 +24023,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>21</v>
       </c>
@@ -24026,7 +24031,7 @@
         <v>131</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>407</v>
@@ -24083,7 +24088,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>21</v>
       </c>
@@ -24091,7 +24096,7 @@
         <v>133</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>408</v>
@@ -24148,7 +24153,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>21</v>
       </c>
@@ -24156,7 +24161,7 @@
         <v>135</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>409</v>
@@ -24213,7 +24218,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>21</v>
       </c>
@@ -24221,7 +24226,7 @@
         <v>137</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>410</v>
@@ -24278,7 +24283,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>21</v>
       </c>
@@ -24286,7 +24291,7 @@
         <v>139</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>411</v>
@@ -24343,7 +24348,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>21</v>
       </c>
@@ -24351,7 +24356,7 @@
         <v>141</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>412</v>
@@ -24408,7 +24413,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>21</v>
       </c>
@@ -24416,7 +24421,7 @@
         <v>143</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>413</v>
@@ -24473,7 +24478,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>21</v>
       </c>
@@ -24481,7 +24486,7 @@
         <v>145</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>414</v>
@@ -24538,7 +24543,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>21</v>
       </c>
@@ -24546,7 +24551,7 @@
         <v>147</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>415</v>
@@ -24603,7 +24608,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>21</v>
       </c>
@@ -24611,7 +24616,7 @@
         <v>149</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>416</v>
@@ -24668,7 +24673,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>21</v>
       </c>
@@ -24676,7 +24681,7 @@
         <v>151</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>417</v>
@@ -24733,7 +24738,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>21</v>
       </c>
@@ -24741,7 +24746,7 @@
         <v>153</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>418</v>
@@ -24798,7 +24803,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>21</v>
       </c>
@@ -24806,7 +24811,7 @@
         <v>155</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>419</v>
@@ -24863,7 +24868,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
         <v>21</v>
       </c>
@@ -24871,7 +24876,7 @@
         <v>157</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>420</v>
@@ -24928,7 +24933,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>21</v>
       </c>
@@ -24936,7 +24941,7 @@
         <v>159</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>421</v>
@@ -24993,7 +24998,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>21</v>
       </c>
@@ -25001,7 +25006,7 @@
         <v>161</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>422</v>
@@ -25058,7 +25063,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>21</v>
       </c>
@@ -25066,7 +25071,7 @@
         <v>163</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>423</v>
@@ -25123,7 +25128,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>21</v>
       </c>
@@ -25131,7 +25136,7 @@
         <v>165</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>424</v>
@@ -25188,7 +25193,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>21</v>
       </c>
@@ -25196,7 +25201,7 @@
         <v>167</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>425</v>
@@ -25253,7 +25258,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>21</v>
       </c>
@@ -25261,7 +25266,7 @@
         <v>169</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>426</v>
@@ -25318,7 +25323,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
         <v>21</v>
       </c>
@@ -25326,7 +25331,7 @@
         <v>171</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>427</v>
@@ -25383,7 +25388,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>21</v>
       </c>
@@ -25391,7 +25396,7 @@
         <v>173</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>428</v>
@@ -25448,7 +25453,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>21</v>
       </c>
@@ -25456,7 +25461,7 @@
         <v>175</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>429</v>
@@ -25513,7 +25518,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>21</v>
       </c>
@@ -25521,7 +25526,7 @@
         <v>177</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>430</v>
@@ -25578,7 +25583,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>21</v>
       </c>
@@ -25586,7 +25591,7 @@
         <v>179</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>431</v>
@@ -25643,7 +25648,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>21</v>
       </c>
@@ -25651,7 +25656,7 @@
         <v>181</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>432</v>
@@ -25708,7 +25713,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>21</v>
       </c>
@@ -25716,7 +25721,7 @@
         <v>183</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>433</v>
@@ -25773,7 +25778,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>21</v>
       </c>
@@ -25781,7 +25786,7 @@
         <v>185</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>434</v>
@@ -25838,7 +25843,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>21</v>
       </c>
@@ -25846,7 +25851,7 @@
         <v>187</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>435</v>
@@ -25903,7 +25908,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="68.65" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
         <v>21</v>
       </c>
@@ -25911,7 +25916,7 @@
         <v>189</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>436</v>
@@ -25968,7 +25973,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
         <v>21</v>
       </c>
@@ -25976,7 +25981,7 @@
         <v>192</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>437</v>
@@ -26033,7 +26038,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
         <v>21</v>
       </c>
@@ -26041,7 +26046,7 @@
         <v>194</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>438</v>
@@ -26098,7 +26103,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>21</v>
       </c>
@@ -26106,7 +26111,7 @@
         <v>196</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>439</v>
@@ -26163,7 +26168,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>21</v>
       </c>
@@ -26171,7 +26176,7 @@
         <v>198</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>440</v>
@@ -26228,7 +26233,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>21</v>
       </c>
@@ -26236,7 +26241,7 @@
         <v>200</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>441</v>
@@ -26293,7 +26298,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>21</v>
       </c>
@@ -26301,7 +26306,7 @@
         <v>202</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>442</v>
@@ -26358,7 +26363,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>21</v>
       </c>
@@ -26366,7 +26371,7 @@
         <v>204</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>443</v>
@@ -26423,7 +26428,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>21</v>
       </c>
@@ -26431,7 +26436,7 @@
         <v>206</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>444</v>
@@ -26488,7 +26493,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>21</v>
       </c>
@@ -26496,7 +26501,7 @@
         <v>208</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>445</v>
@@ -26553,7 +26558,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="79.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
         <v>21</v>
       </c>
@@ -26561,7 +26566,7 @@
         <v>210</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>446</v>
@@ -26618,7 +26623,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
         <v>21</v>
       </c>
@@ -26626,7 +26631,7 @@
         <v>212</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>447</v>
@@ -26683,7 +26688,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
         <v>21</v>
       </c>
@@ -26691,7 +26696,7 @@
         <v>214</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>448</v>
@@ -26748,7 +26753,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
         <v>21</v>
       </c>
@@ -26756,7 +26761,7 @@
         <v>216</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>449</v>
@@ -26813,7 +26818,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
         <v>21</v>
       </c>
@@ -26821,7 +26826,7 @@
         <v>218</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>450</v>
@@ -26878,7 +26883,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
         <v>21</v>
       </c>
@@ -26886,7 +26891,7 @@
         <v>220</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>451</v>
@@ -26943,7 +26948,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
         <v>21</v>
       </c>
@@ -26951,7 +26956,7 @@
         <v>222</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>452</v>
@@ -27008,7 +27013,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
         <v>21</v>
       </c>
@@ -27016,7 +27021,7 @@
         <v>224</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>453</v>
@@ -27073,7 +27078,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
         <v>21</v>
       </c>
@@ -27081,7 +27086,7 @@
         <v>226</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>454</v>
@@ -27138,7 +27143,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
         <v>21</v>
       </c>
@@ -27146,7 +27151,7 @@
         <v>228</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>455</v>
@@ -27203,7 +27208,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
         <v>21</v>
       </c>
@@ -27211,7 +27216,7 @@
         <v>230</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>456</v>
@@ -27268,7 +27273,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
         <v>21</v>
       </c>
@@ -27276,7 +27281,7 @@
         <v>232</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>457</v>
@@ -27333,7 +27338,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
         <v>21</v>
       </c>
@@ -27341,7 +27346,7 @@
         <v>234</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>458</v>
@@ -27398,7 +27403,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
         <v>21</v>
       </c>
@@ -27406,7 +27411,7 @@
         <v>236</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>459</v>
@@ -27463,7 +27468,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
         <v>21</v>
       </c>
@@ -27471,7 +27476,7 @@
         <v>238</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>460</v>
@@ -27528,7 +27533,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
         <v>21</v>
       </c>
@@ -27536,7 +27541,7 @@
         <v>240</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>461</v>
@@ -27593,7 +27598,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
         <v>21</v>
       </c>
@@ -27601,7 +27606,7 @@
         <v>242</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>462</v>
@@ -27658,7 +27663,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
         <v>21</v>
       </c>
@@ -27666,7 +27671,7 @@
         <v>244</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>463</v>
@@ -27723,7 +27728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
         <v>21</v>
       </c>
@@ -27731,7 +27736,7 @@
         <v>246</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>464</v>
@@ -27788,7 +27793,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
         <v>21</v>
       </c>
@@ -27796,7 +27801,7 @@
         <v>248</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>465</v>
@@ -27853,7 +27858,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
         <v>21</v>
       </c>
@@ -27861,7 +27866,7 @@
         <v>250</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>466</v>
@@ -27918,7 +27923,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
         <v>21</v>
       </c>
@@ -27926,7 +27931,7 @@
         <v>252</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>467</v>
@@ -27983,7 +27988,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
         <v>21</v>
       </c>
@@ -27991,7 +27996,7 @@
         <v>254</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>468</v>
@@ -28048,7 +28053,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
         <v>21</v>
       </c>
@@ -28056,7 +28061,7 @@
         <v>256</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>469</v>
@@ -28113,7 +28118,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
         <v>21</v>
       </c>
@@ -28121,7 +28126,7 @@
         <v>258</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>470</v>
@@ -28178,7 +28183,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
         <v>21</v>
       </c>
@@ -28186,7 +28191,7 @@
         <v>260</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>471</v>
@@ -28243,7 +28248,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
         <v>21</v>
       </c>
@@ -28251,7 +28256,7 @@
         <v>262</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>472</v>
@@ -28308,7 +28313,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
         <v>21</v>
       </c>
@@ -28316,7 +28321,7 @@
         <v>264</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>473</v>
@@ -28373,7 +28378,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
         <v>21</v>
       </c>
@@ -28381,7 +28386,7 @@
         <v>266</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>474</v>
@@ -28438,7 +28443,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
         <v>21</v>
       </c>
@@ -28446,7 +28451,7 @@
         <v>268</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>475</v>
@@ -28503,7 +28508,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
         <v>21</v>
       </c>
@@ -28511,7 +28516,7 @@
         <v>270</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>476</v>
@@ -28568,7 +28573,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="91" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
         <v>21</v>
       </c>
@@ -28576,7 +28581,7 @@
         <v>272</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>477</v>
@@ -28633,7 +28638,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
         <v>21</v>
       </c>
@@ -28641,7 +28646,7 @@
         <v>274</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>478</v>
@@ -28698,7 +28703,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
         <v>21</v>
       </c>
@@ -28706,7 +28711,7 @@
         <v>276</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>479</v>
@@ -28763,7 +28768,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
         <v>21</v>
       </c>
@@ -28771,7 +28776,7 @@
         <v>278</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>480</v>
@@ -28828,7 +28833,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
         <v>21</v>
       </c>
@@ -28836,7 +28841,7 @@
         <v>280</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>481</v>
@@ -28893,7 +28898,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
         <v>21</v>
       </c>
@@ -28901,7 +28906,7 @@
         <v>282</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>482</v>
@@ -28958,7 +28963,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
         <v>21</v>
       </c>
@@ -28966,7 +28971,7 @@
         <v>284</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>483</v>
@@ -29023,7 +29028,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
         <v>21</v>
       </c>
@@ -29031,7 +29036,7 @@
         <v>286</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>484</v>
@@ -29088,7 +29093,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
         <v>21</v>
       </c>
@@ -29096,7 +29101,7 @@
         <v>288</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>485</v>
@@ -29153,7 +29158,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
         <v>21</v>
       </c>
@@ -29161,7 +29166,7 @@
         <v>290</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>486</v>
@@ -29218,7 +29223,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="102.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
         <v>21</v>
       </c>
@@ -29226,7 +29231,7 @@
         <v>292</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>487</v>
@@ -29283,7 +29288,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
         <v>21</v>
       </c>
@@ -29291,7 +29296,7 @@
         <v>294</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>488</v>
@@ -29348,7 +29353,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
         <v>21</v>
       </c>
@@ -29356,7 +29361,7 @@
         <v>296</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>489</v>
@@ -29413,7 +29418,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
         <v>21</v>
       </c>
@@ -29421,7 +29426,7 @@
         <v>298</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>490</v>
@@ -29478,7 +29483,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
         <v>21</v>
       </c>
@@ -29486,7 +29491,7 @@
         <v>300</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>491</v>
@@ -29543,7 +29548,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>21</v>
       </c>
@@ -29551,7 +29556,7 @@
         <v>302</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>492</v>
@@ -29608,7 +29613,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
         <v>21</v>
       </c>
@@ -29616,7 +29621,7 @@
         <v>304</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>493</v>
@@ -29673,7 +29678,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
         <v>21</v>
       </c>
@@ -29681,7 +29686,7 @@
         <v>306</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>494</v>
@@ -29738,7 +29743,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
         <v>21</v>
       </c>
@@ -29746,7 +29751,7 @@
         <v>308</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>495</v>
@@ -29803,7 +29808,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
         <v>21</v>
       </c>
@@ -29811,7 +29816,7 @@
         <v>310</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>496</v>
@@ -29868,7 +29873,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
         <v>21</v>
       </c>
@@ -29876,7 +29881,7 @@
         <v>312</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>497</v>
@@ -29933,7 +29938,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
         <v>21</v>
       </c>
@@ -29941,7 +29946,7 @@
         <v>314</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>498</v>
@@ -29998,7 +30003,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
         <v>21</v>
       </c>
@@ -30006,7 +30011,7 @@
         <v>316</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>499</v>
@@ -30063,7 +30068,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
         <v>21</v>
       </c>
@@ -30071,7 +30076,7 @@
         <v>318</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>500</v>
@@ -30128,7 +30133,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
         <v>21</v>
       </c>
@@ -30136,7 +30141,7 @@
         <v>320</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>501</v>
@@ -30193,7 +30198,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
         <v>21</v>
       </c>
@@ -30201,7 +30206,7 @@
         <v>322</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>502</v>
@@ -30258,7 +30263,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
         <v>21</v>
       </c>
@@ -30266,7 +30271,7 @@
         <v>324</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>503</v>
@@ -30323,7 +30328,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
         <v>21</v>
       </c>
@@ -30331,7 +30336,7 @@
         <v>326</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>504</v>
@@ -30388,7 +30393,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
         <v>21</v>
       </c>
@@ -30396,7 +30401,7 @@
         <v>328</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>505</v>
@@ -30453,7 +30458,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
         <v>21</v>
       </c>
@@ -30461,7 +30466,7 @@
         <v>330</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>506</v>
@@ -30518,7 +30523,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
         <v>21</v>
       </c>
@@ -30526,7 +30531,7 @@
         <v>332</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>507</v>
@@ -30583,7 +30588,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
         <v>21</v>
       </c>
@@ -30591,7 +30596,7 @@
         <v>334</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>508</v>
@@ -30648,7 +30653,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
         <v>21</v>
       </c>
@@ -30656,7 +30661,7 @@
         <v>336</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>509</v>
@@ -30713,7 +30718,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
         <v>21</v>
       </c>
@@ -30721,7 +30726,7 @@
         <v>338</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>510</v>
@@ -30778,7 +30783,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
         <v>21</v>
       </c>
@@ -30786,7 +30791,7 @@
         <v>340</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>511</v>
@@ -30843,7 +30848,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
         <v>21</v>
       </c>
@@ -30851,7 +30856,7 @@
         <v>342</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>512</v>
@@ -30908,7 +30913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
         <v>21</v>
       </c>
@@ -30916,7 +30921,7 @@
         <v>344</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D161" s="1" t="s">
         <v>513</v>
@@ -30973,7 +30978,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
         <v>21</v>
       </c>
@@ -30981,7 +30986,7 @@
         <v>346</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D162" s="1" t="s">
         <v>514</v>
@@ -31038,7 +31043,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
         <v>21</v>
       </c>
@@ -31046,7 +31051,7 @@
         <v>348</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>515</v>
@@ -31103,7 +31108,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
         <v>21</v>
       </c>
@@ -31111,7 +31116,7 @@
         <v>350</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>516</v>
@@ -31168,7 +31173,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
         <v>21</v>
       </c>
@@ -31176,7 +31181,7 @@
         <v>352</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>517</v>
@@ -31234,6 +31239,28 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:U165">
+    <filterColumn colId="5">
+      <customFilters and="true">
+        <customFilter operator="equal" val="Calendar Year"/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="10">
+      <customFilters and="true">
+        <customFilter operator="equal" val="Yes"/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="15">
+      <customFilters and="true">
+        <customFilter operator="equal" val="No"/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="8">
+      <customFilters and="true">
+        <customFilter operator="equal" val="No"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -31241,6 +31268,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -31259,12 +31287,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.5"/>
-    <col collapsed="false" hidden="false" max="20" min="5" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="20" min="5" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36455,13 +36483,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.5"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41883,9 +41911,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -47307,11 +47335,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="7" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="20.25"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="7" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52733,9 +52761,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="48.3265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="47.6530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -58157,13 +58185,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.5"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -71775,9 +71803,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>